<commit_message>
Worked on adding Keyword validation
- updated file names
- started a class to validate keywords
- added browser radio group to dialog and renamed class
</commit_message>
<xml_diff>
--- a/Dragonfly/Tools/dragonfly.xlsx
+++ b/Dragonfly/Tools/dragonfly.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="test_configuration" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="test_elements" sheetId="3" r:id="rId3"/>
     <sheet name="test_instances" sheetId="4" r:id="rId4"/>
     <sheet name="test_modules" sheetId="5" r:id="rId5"/>
+    <sheet name="Keywords" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t xml:space="preserve">test_details: </t>
   </si>
@@ -108,15 +109,94 @@
   </si>
   <si>
     <t>key_value</t>
+  </si>
+  <si>
+    <t>&lt;td&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ti&gt;</t>
+  </si>
+  <si>
+    <t>&lt;tl&gt;</t>
+  </si>
+  <si>
+    <t>&lt;te&gt;</t>
+  </si>
+  <si>
+    <t>&lt;re&gt;</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>&lt;if&gt;</t>
+  </si>
+  <si>
+    <t>&lt;else if&gt;</t>
+  </si>
+  <si>
+    <t>&lt;else&gt;</t>
+  </si>
+  <si>
+    <t>&lt;end if&gt;</t>
+  </si>
+  <si>
+    <t>&lt;loopexit&gt;</t>
+  </si>
+  <si>
+    <t>&lt;loopend&gt;</t>
+  </si>
+  <si>
+    <t>&lt;loopstart&gt;</t>
+  </si>
+  <si>
+    <t>&lt;click&gt;</t>
+  </si>
+  <si>
+    <t>&lt;doubleclick&gt;</t>
+  </si>
+  <si>
+    <t>&lt;rightclick&gt;</t>
+  </si>
+  <si>
+    <t>&lt;on&gt;</t>
+  </si>
+  <si>
+    <t>&lt;off&gt;</t>
+  </si>
+  <si>
+    <t>&lt;blank&gt;</t>
+  </si>
+  <si>
+    <t>&lt;first&gt;</t>
+  </si>
+  <si>
+    <t>&lt;second&gt;</t>
+  </si>
+  <si>
+    <t>&lt;third&gt;</t>
+  </si>
+  <si>
+    <t>&lt;last&gt;</t>
+  </si>
+  <si>
+    <t>&lt;random&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -164,10 +244,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -625,13 +706,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,24 +799,60 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -743,15 +860,21 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="N3" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -764,15 +887,21 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="N4" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -785,15 +914,21 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -807,14 +942,18 @@
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -828,14 +967,18 @@
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -849,14 +992,18 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -870,7 +1017,9 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -891,7 +1040,9 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -912,7 +1063,9 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -933,7 +1086,9 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -947,8 +1102,147 @@
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
     </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A4" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:A5">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>